<commit_message>
add new results to excel sheet
</commit_message>
<xml_diff>
--- a/ECO_RESULTS.xlsx
+++ b/ECO_RESULTS.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ROSSA\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\40204617\IdeaProjects\emergent_computing_cw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AB5B5269-C731-400A-9F3E-841F18E4D85A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{57BE1560-0062-43FD-80B3-C6D9C9296EBF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>EA Type</t>
   </si>
@@ -105,13 +104,37 @@
   </si>
   <si>
     <t>FitnessSharing Theshold 7</t>
+  </si>
+  <si>
+    <t>MixedTsEA_pop_150_tsize_10</t>
+  </si>
+  <si>
+    <t>MixedTsEA_pop_150_tsize_20</t>
+  </si>
+  <si>
+    <t>MixedTsEA_pop_150_tsize_30</t>
+  </si>
+  <si>
+    <t>MixedTsEA_pop_150_tsize_40</t>
+  </si>
+  <si>
+    <t>MixedTsEA_pop_150_tsize_50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OnePointTsEA </t>
+  </si>
+  <si>
+    <t>TwoPointTsEA</t>
+  </si>
+  <si>
+    <t>FitnessSharing Theshold 3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -122,6 +145,12 @@
     <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="7.2"/>
+      <color rgb="FFA9B7C6"/>
       <name val="Courier New"/>
       <family val="3"/>
     </font>
@@ -146,9 +175,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -464,21 +496,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE8D2391-BA04-4D4D-83E3-CC79B4F1D6B4}">
-  <dimension ref="A1:M14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.1796875" customWidth="1"/>
-    <col min="12" max="12" width="15.6328125" customWidth="1"/>
+    <col min="1" max="1" width="26.21875" customWidth="1"/>
+    <col min="12" max="12" width="15.6640625" customWidth="1"/>
     <col min="13" max="13" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -519,7 +551,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -562,7 +594,7 @@
         <v>2.840373653236488</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -605,7 +637,7 @@
         <v>1.0139851872685266</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -648,7 +680,7 @@
         <v>1.4223223966457177</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -691,7 +723,7 @@
         <v>2.0693138959568222</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -734,7 +766,7 @@
         <v>1.599731539977878</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -777,7 +809,7 @@
         <v>0.96378754920366305</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -820,7 +852,7 @@
         <v>1.3259068594739234</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -863,176 +895,283 @@
         <v>1.2510501828463954</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="1">
-        <v>215.68200000001201</v>
-      </c>
-      <c r="C11" s="1">
-        <v>213.78200000000001</v>
-      </c>
-      <c r="D11" s="1">
-        <v>213.78200000000001</v>
-      </c>
-      <c r="E11" s="1">
-        <v>215.11799999999999</v>
-      </c>
-      <c r="F11" s="1">
-        <v>216.96</v>
-      </c>
-      <c r="G11" s="1">
-        <v>216.96</v>
-      </c>
-      <c r="H11" s="1">
-        <v>216.20599999999999</v>
-      </c>
-      <c r="I11" s="1">
-        <v>216.20599999999999</v>
-      </c>
-      <c r="J11" s="1">
-        <v>215.11799999999999</v>
-      </c>
-      <c r="K11" s="1">
-        <v>215.11799999999999</v>
-      </c>
-      <c r="L11">
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" t="e">
         <f>AVERAGE(B11:K11)</f>
-        <v>215.4932000000012</v>
-      </c>
-      <c r="M11">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M11" t="e">
         <f>_xlfn.STDEV.P(B11:K11)</f>
-        <v>1.0785895234056599</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="1">
-        <v>215.870000000012</v>
-      </c>
-      <c r="C12" s="1">
-        <v>215.87</v>
-      </c>
-      <c r="D12" s="1">
-        <v>215.87</v>
-      </c>
-      <c r="E12" s="1">
-        <v>215.084</v>
-      </c>
-      <c r="F12" s="1">
-        <v>215.41399999999999</v>
-      </c>
-      <c r="G12" s="1">
-        <v>215.28</v>
-      </c>
-      <c r="H12" s="1">
-        <v>214.16800000000001</v>
-      </c>
-      <c r="I12" s="1">
-        <v>214.16800000000001</v>
-      </c>
-      <c r="J12" s="1">
-        <v>214.16800000000001</v>
-      </c>
-      <c r="K12" s="1">
-        <v>214.16800000000001</v>
-      </c>
-      <c r="L12">
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" t="e">
         <f>AVERAGE(B12:K12)</f>
-        <v>215.00600000000122</v>
-      </c>
-      <c r="M12">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M12" t="e">
         <f>_xlfn.STDEV.P(B12:K12)</f>
-        <v>0.7277422620695253</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="1">
-        <v>217.34</v>
-      </c>
-      <c r="C13" s="1">
-        <v>217.34</v>
-      </c>
-      <c r="D13" s="1">
-        <v>217.34</v>
-      </c>
-      <c r="E13" s="1">
-        <v>217.34</v>
-      </c>
-      <c r="F13" s="1">
-        <v>217.22800000000001</v>
-      </c>
-      <c r="G13" s="1">
-        <v>217.22800000000001</v>
-      </c>
-      <c r="H13" s="1">
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" t="e">
+        <f>AVERAGE(B13:K13)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M13" t="e">
+        <f>_xlfn.STDEV.P(B13:K13)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" t="e">
+        <f>AVERAGE(B14:K14)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M14" t="e">
+        <f>_xlfn.STDEV.P(B14:K14)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16">
+        <v>216.58</v>
+      </c>
+      <c r="C16">
+        <v>214.15</v>
+      </c>
+      <c r="D16">
+        <v>214.85</v>
+      </c>
+      <c r="E16">
+        <v>213.82599999999999</v>
+      </c>
+      <c r="F16">
+        <v>215.8</v>
+      </c>
+      <c r="G16">
+        <v>214.51</v>
+      </c>
+      <c r="H16">
+        <v>214.3</v>
+      </c>
+      <c r="I16">
+        <v>215.64</v>
+      </c>
+      <c r="J16">
+        <v>213.74</v>
+      </c>
+      <c r="K16">
+        <v>216.15</v>
+      </c>
+      <c r="L16">
+        <f t="shared" ref="L16" si="2">AVERAGE(B16:K16)</f>
+        <v>214.95459999999997</v>
+      </c>
+      <c r="M16">
+        <f t="shared" ref="M16" si="3">_xlfn.STDEV.P(B16:K16)</f>
+        <v>0.96378754920366305</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="2">
+        <v>215.50400000001099</v>
+      </c>
+      <c r="C17" s="2">
+        <v>215.58600000001201</v>
+      </c>
+      <c r="D17" s="2">
+        <v>215.03400000001201</v>
+      </c>
+      <c r="E17" s="2">
+        <v>214.67400000001399</v>
+      </c>
+      <c r="F17" s="2">
+        <v>212.364000000012</v>
+      </c>
+      <c r="G17" s="2">
+        <v>214.02800000001099</v>
+      </c>
+      <c r="H17" s="2">
+        <v>216.900000000012</v>
+      </c>
+      <c r="I17" s="2">
+        <v>212.65800000001099</v>
+      </c>
+      <c r="J17" s="2">
+        <v>215.06200000001101</v>
+      </c>
+      <c r="K17" s="2">
+        <v>212.118000000009</v>
+      </c>
+      <c r="L17">
+        <f>AVERAGE(B17:K17)</f>
+        <v>214.3928000000115</v>
+      </c>
+      <c r="M17">
+        <f>_xlfn.STDEV.P(B17:K17)</f>
+        <v>1.4938519873138527</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="2">
+        <v>214.79</v>
+      </c>
+      <c r="C18" s="2">
+        <v>215.172</v>
+      </c>
+      <c r="D18" s="2">
+        <v>214.80600000000001</v>
+      </c>
+      <c r="E18" s="2">
+        <v>213.96199999999999</v>
+      </c>
+      <c r="F18" s="2">
+        <v>215.352</v>
+      </c>
+      <c r="G18" s="2">
+        <v>213.398</v>
+      </c>
+      <c r="H18" s="2">
+        <v>213.68600000000001</v>
+      </c>
+      <c r="I18" s="2">
+        <v>214.04599999999999</v>
+      </c>
+      <c r="J18" s="2">
+        <v>215.452</v>
+      </c>
+      <c r="K18">
+        <v>217.84899999999999</v>
+      </c>
+      <c r="L18">
+        <f>AVERAGE(B18:K18)</f>
+        <v>214.85129999999998</v>
+      </c>
+      <c r="M18">
+        <f>_xlfn.STDEV.P(B18:K18)</f>
+        <v>1.2089570753339411</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="2">
+        <v>215.452</v>
+      </c>
+      <c r="C19" s="2">
+        <v>217.84899999999999</v>
+      </c>
+      <c r="D19" s="2">
+        <v>217.15899999999999</v>
+      </c>
+      <c r="E19" s="2">
         <v>215.35599999999999</v>
       </c>
-      <c r="I13" s="1">
-        <v>215.35599999999999</v>
-      </c>
-      <c r="J13" s="1">
-        <v>215.35599999999999</v>
-      </c>
-      <c r="K13" s="1">
-        <v>215.35599999999999</v>
-      </c>
-      <c r="L13">
-        <f>AVERAGE(B13:K13)</f>
-        <v>216.52399999999997</v>
-      </c>
-      <c r="M13">
-        <f>_xlfn.STDEV.P(B13:K13)</f>
-        <v>0.95454449870082536</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" s="1">
-        <v>217.65899999999999</v>
-      </c>
-      <c r="C14" s="1">
-        <v>217.65899999999999</v>
-      </c>
-      <c r="D14" s="1">
-        <v>215.24799999999999</v>
-      </c>
-      <c r="E14" s="1">
-        <v>215.24799999999999</v>
-      </c>
-      <c r="F14" s="1">
-        <v>215.11799999999999</v>
-      </c>
-      <c r="G14" s="1">
-        <v>215.11799999999999</v>
-      </c>
-      <c r="H14" s="1">
-        <v>215.11799999999999</v>
-      </c>
-      <c r="I14" s="1">
-        <v>215.11799999999999</v>
-      </c>
-      <c r="J14" s="1">
-        <v>215.11799999999999</v>
-      </c>
-      <c r="K14" s="1">
-        <v>217.65899999999999</v>
-      </c>
-      <c r="L14">
-        <f>AVERAGE(B14:K14)</f>
-        <v>215.90629999999996</v>
-      </c>
-      <c r="M14">
-        <f>_xlfn.STDEV.P(B14:K14)</f>
-        <v>1.1484630642732914</v>
+      <c r="F19" s="2">
+        <v>219.71299999999999</v>
+      </c>
+      <c r="G19" s="2">
+        <v>217.096</v>
+      </c>
+      <c r="H19" s="2">
+        <v>217.81399999999999</v>
+      </c>
+      <c r="I19" s="2">
+        <v>217.822</v>
+      </c>
+      <c r="J19">
+        <v>213.93199999999999</v>
+      </c>
+      <c r="K19" s="2">
+        <v>214.72</v>
+      </c>
+      <c r="L19">
+        <f>AVERAGE(B19:K19)</f>
+        <v>216.69130000000001</v>
+      </c>
+      <c r="M19">
+        <f>_xlfn.STDEV.P(B19:K19)</f>
+        <v>1.6796146611648761</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>